<commit_message>
Q1.8 Perform tests and update
</commit_message>
<xml_diff>
--- a/part1/JSAT2-Part1-Test-plan.xlsx
+++ b/part1/JSAT2-Part1-Test-plan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Test Result (Pass/Fail/Not Executed)</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
   <si>
     <t>Step #</t>
@@ -55,10 +58,16 @@
     <t>App opens in browser</t>
   </si>
   <si>
+    <t>App opened in browser</t>
+  </si>
+  <si>
     <t>verify JS file is correctly linked to html file using console.log</t>
   </si>
   <si>
     <t>console.log("test"); will display "test" in browser console</t>
+  </si>
+  <si>
+    <t>"test" was displayed in console</t>
   </si>
   <si>
     <t>call sequentialSearch function with an array and a target that does exist in the array</t>
@@ -67,16 +76,34 @@
     <t>console will display a positive integer of the index of the target in the array</t>
   </si>
   <si>
+    <t>console displayed "9" as the index of the target number, which was 10th item in the array</t>
+  </si>
+  <si>
     <t>repeat step 3 with a target that does not exist within the array</t>
   </si>
   <si>
     <t>console will display -1 as the target is not found</t>
   </si>
   <si>
+    <t>console displayed "-1" as the target did not exist in the array</t>
+  </si>
+  <si>
     <t>call binarySearch function with an array and a target that does exist in the array</t>
   </si>
   <si>
+    <t>console will display the sorted array and a positive integer of the index of the target in the array</t>
+  </si>
+  <si>
+    <t>Console output the array as sorted and "5" as the index (for a target number which was the 6th item in the array)</t>
+  </si>
+  <si>
     <t>repeat step 5 with a target that does not exist within the array</t>
+  </si>
+  <si>
+    <t>console will display the sorted array and -1 as the target is not found</t>
+  </si>
+  <si>
+    <t>Console output the array as sorted and "-1" as the target did not exist in the array</t>
   </si>
 </sst>
 </file>
@@ -306,7 +333,7 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -327,12 +354,14 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -554,7 +583,8 @@
     <col customWidth="1" min="3" max="3" width="8.88"/>
     <col customWidth="1" min="4" max="4" width="9.13"/>
     <col customWidth="1" min="5" max="5" width="19.13"/>
-    <col customWidth="1" min="6" max="8" width="9.13"/>
+    <col customWidth="1" min="6" max="7" width="9.13"/>
+    <col customWidth="1" min="8" max="8" width="11.0"/>
     <col customWidth="1" min="9" max="9" width="32.38"/>
     <col customWidth="1" min="10" max="10" width="9.13"/>
     <col customWidth="1" min="11" max="11" width="9.0"/>
@@ -645,7 +675,9 @@
         <v>6</v>
       </c>
       <c r="I3" s="10"/>
-      <c r="J3" s="13"/>
+      <c r="J3" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="K3" s="6"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
@@ -693,23 +725,23 @@
     </row>
     <row r="5">
       <c r="A5" s="14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="16"/>
       <c r="I5" s="15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J5" s="18"/>
       <c r="K5" s="16"/>
@@ -762,17 +794,21 @@
         <v>1.0</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="24"/>
+      <c r="F7" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="24"/>
+      <c r="I7" s="24" t="s">
+        <v>7</v>
+      </c>
       <c r="J7" s="5"/>
       <c r="K7" s="6"/>
       <c r="L7" s="7"/>
@@ -796,17 +832,21 @@
         <v>2.0</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="24"/>
+      <c r="F8" s="24" t="s">
+        <v>18</v>
+      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="24"/>
+      <c r="I8" s="24" t="s">
+        <v>7</v>
+      </c>
       <c r="J8" s="5"/>
       <c r="K8" s="6"/>
       <c r="L8" s="7"/>
@@ -830,17 +870,21 @@
         <v>3.0</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="24"/>
+      <c r="F9" s="24" t="s">
+        <v>21</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="24"/>
+      <c r="I9" s="24" t="s">
+        <v>7</v>
+      </c>
       <c r="J9" s="5"/>
       <c r="K9" s="6"/>
       <c r="L9" s="7"/>
@@ -864,17 +908,21 @@
         <v>4.0</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="24"/>
+      <c r="F10" s="24" t="s">
+        <v>24</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="24"/>
+      <c r="I10" s="24" t="s">
+        <v>7</v>
+      </c>
       <c r="J10" s="5"/>
       <c r="K10" s="6"/>
       <c r="L10" s="7"/>
@@ -898,17 +946,21 @@
         <v>5.0</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="24"/>
+      <c r="F11" s="24" t="s">
+        <v>27</v>
+      </c>
       <c r="G11" s="5"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="24"/>
+      <c r="I11" s="24" t="s">
+        <v>7</v>
+      </c>
       <c r="J11" s="5"/>
       <c r="K11" s="6"/>
       <c r="L11" s="7"/>
@@ -932,17 +984,21 @@
         <v>6.0</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="26"/>
+      <c r="F12" s="24" t="s">
+        <v>30</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="26"/>
+      <c r="I12" s="26" t="s">
+        <v>7</v>
+      </c>
       <c r="J12" s="5"/>
       <c r="K12" s="6"/>
       <c r="L12" s="7"/>

</xml_diff>